<commit_message>
bf: update tas forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/2023/september/bf_lf_tas1_202309_2_participant.xlsx
+++ b/LF/TAS/Burkina Faso/2023/september/bf_lf_tas1_202309_2_participant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2023\september\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA67B9D-0089-424C-B63F-0ECE3861D245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789B0E32-A327-47CB-B703-86B96644643F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="104">
   <si>
     <t>form_title</t>
   </si>
@@ -283,15 +283,6 @@
     <t>CP2</t>
   </si>
   <si>
-    <t>Séléctionner la classe</t>
-  </si>
-  <si>
-    <t>select_one classe</t>
-  </si>
-  <si>
-    <t>p_classe</t>
-  </si>
-  <si>
     <t>Sélectionnez le nom du CSPS</t>
   </si>
   <si>
@@ -343,10 +334,22 @@
     <t>p_recu_avm_alb</t>
   </si>
   <si>
-    <t>bf_lf_tas1_202309_2_participant</t>
-  </si>
-  <si>
-    <t>(Sept 2023) Burkina Faso TAS FL - 2. Formulaire Enrôlement</t>
+    <t>(Sept 2023) Burkina Faso TAS FL - 2. Formulaire Enrôlement V2</t>
+  </si>
+  <si>
+    <t>bf_lf_tas1_202309_2_participant_v2</t>
+  </si>
+  <si>
+    <t>Allez à la question suivante</t>
+  </si>
+  <si>
+    <t>Type de TAS</t>
+  </si>
+  <si>
+    <t>p_type_tas</t>
+  </si>
+  <si>
+    <t>${p_type_tas} = 'TAS1'</t>
   </si>
 </sst>
 </file>
@@ -849,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -974,10 +977,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -995,7 +998,7 @@
         <v>77</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1010,10 +1013,10 @@
         <v>27</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1023,87 +1026,104 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="7"/>
+      <c r="A10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="H11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="G12" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>72</v>
+      <c r="E13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>58</v>
@@ -1113,47 +1133,45 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>58</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="7" t="s">
@@ -1161,23 +1179,18 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>91</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1185,14 +1198,14 @@
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>29</v>
+      <c r="A17" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1202,81 +1215,65 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="H18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
+      <c r="A20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1365,10 +1362,10 @@
         <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D6" s="12"/>
     </row>
@@ -1377,10 +1374,10 @@
         <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D7" s="12"/>
     </row>
@@ -1398,7 +1395,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1410,7 +1407,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1708,7 +1705,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1733,10 +1730,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>

</xml_diff>